<commit_message>
BEQI test bug fixed
</commit_message>
<xml_diff>
--- a/scoring/tests/BEQI/BEQI93_test_1.xlsx
+++ b/scoring/tests/BEQI/BEQI93_test_1.xlsx
@@ -450,7 +450,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -500,7 +500,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -520,7 +520,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -560,7 +560,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -580,7 +580,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -620,7 +620,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -660,7 +660,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -680,7 +680,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -730,7 +730,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -740,7 +740,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -760,7 +760,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -770,7 +770,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -780,7 +780,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -790,7 +790,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -800,7 +800,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -810,7 +810,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -840,7 +840,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -850,7 +850,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -860,7 +860,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -880,7 +880,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -890,7 +890,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -900,7 +900,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -920,7 +920,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -940,7 +940,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -950,7 +950,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -960,7 +960,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -990,7 +990,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1250,7 +1250,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1260,7 +1260,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1300,7 +1300,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
@@ -1502,7 +1502,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16">
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -1522,7 +1522,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19">
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20">
@@ -1552,7 +1552,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21">
@@ -1562,7 +1562,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>